<commit_message>
Parallel Colt statistics tests
</commit_message>
<xml_diff>
--- a/test/colt/VALE3_short.xlsx
+++ b/test/colt/VALE3_short.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -40,9 +40,6 @@
     <t>durbin watson</t>
   </si>
   <si>
-    <t>frequencies</t>
-  </si>
-  <si>
     <t>geometric mean</t>
   </si>
   <si>
@@ -115,18 +112,12 @@
     <t>skew</t>
   </si>
   <si>
-    <t>split</t>
-  </si>
-  <si>
     <t>sum of squares</t>
   </si>
   <si>
     <t>sum of squared deviations</t>
   </si>
   <si>
-    <t>trimmed mean</t>
-  </si>
-  <si>
     <t>variance</t>
   </si>
   <si>
@@ -148,9 +139,6 @@
     <t>standard error</t>
   </si>
   <si>
-    <t>standardize</t>
-  </si>
-  <si>
     <t>sum</t>
   </si>
   <si>
@@ -172,9 +160,6 @@
     <t>auto correlation (10)</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -223,20 +208,51 @@
     <t>open - log</t>
   </si>
   <si>
-    <t>sum of power deviations(mean, 2)</t>
-  </si>
-  <si>
     <t>(open - mean)^2</t>
   </si>
   <si>
-    <t>sum of powers (2.0)</t>
+    <t>?</t>
+  </si>
+  <si>
+    <t>weighted sum</t>
+  </si>
+  <si>
+    <t>weighted sum of squares</t>
+  </si>
+  <si>
+    <t>weights</t>
+  </si>
+  <si>
+    <t>weighted 
+sum of squares</t>
+  </si>
+  <si>
+    <t>Standardized</t>
+  </si>
+  <si>
+    <t>sum of power deviations(2, mean)</t>
+  </si>
+  <si>
+    <t>sum of powers (3.0)</t>
+  </si>
+  <si>
+    <t>trimmed mean(2, 2)</t>
+  </si>
+  <si>
+    <t>open^3</t>
+  </si>
+  <si>
+    <t>trimmed</t>
+  </si>
+  <si>
+    <t>winzorized</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +384,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -714,13 +738,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1056,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1076,38 +1104,62 @@
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18">
+    <row r="1" spans="2:25" ht="30">
       <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" t="s">
-        <v>60</v>
-      </c>
       <c r="P1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="2:18">
+      <c r="W1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1136,11 +1188,11 @@
         <v>4</v>
       </c>
       <c r="L2">
-        <f>-3+K22/(I33^4)</f>
+        <f>-3+K22/(I32^4)</f>
         <v>-0.92564422252414147</v>
       </c>
     </row>
-    <row r="3" spans="2:18">
+    <row r="3" spans="2:25">
       <c r="B3" s="1">
         <v>41388</v>
       </c>
@@ -1163,19 +1215,19 @@
         <v>33.58</v>
       </c>
       <c r="J3">
-        <f>(C3-$C$34)^$J$2</f>
+        <f t="shared" ref="J3:J21" si="0">(C3-$C$33)^$J$2</f>
         <v>-2.207602230646015E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K21" si="0">(C3-$C$34)^$K$2</f>
+        <f t="shared" ref="K3:K21" si="1">(C3-$C$33)^$K$2</f>
         <v>6.1929052049176439E-3</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M21" si="1">C3-$C$34</f>
+        <f t="shared" ref="M3:M21" si="2">C3-$C$33</f>
         <v>-0.28052631578947995</v>
       </c>
       <c r="N3">
-        <f>D3-$D$34</f>
+        <f>D3-$D$35</f>
         <v>-0.11684210526316008</v>
       </c>
       <c r="O3">
@@ -1194,8 +1246,35 @@
         <f>M3^2</f>
         <v>7.8695013850419035E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:18">
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f>S3*C3</f>
+        <v>33.58</v>
+      </c>
+      <c r="U3">
+        <f>S3*C3*C3</f>
+        <v>1127.6163999999999</v>
+      </c>
+      <c r="V3">
+        <f>(C3-$C$33)/$I$32</f>
+        <v>-0.22351044017086383</v>
+      </c>
+      <c r="W3">
+        <f>C3*C3*C3</f>
+        <v>37865.358711999994</v>
+      </c>
+      <c r="X3">
+        <f>C3</f>
+        <v>33.58</v>
+      </c>
+      <c r="Y3">
+        <f>C3</f>
+        <v>33.58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25">
       <c r="B4" s="1">
         <v>41387</v>
       </c>
@@ -1218,19 +1297,19 @@
         <v>33.4</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J21" si="2">(C4-$C$34)^$J$2</f>
+        <f t="shared" si="0"/>
         <v>-2.3554311054089698</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1339630707757324</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.3305263157894771</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N21" si="3">D4-$D$34</f>
+        <f t="shared" ref="N4:N21" si="3">D4-$D$35</f>
         <v>-0.94684210526315837</v>
       </c>
       <c r="O4">
@@ -1246,11 +1325,38 @@
         <v>3.48216274048526</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R22" si="7">M4^2</f>
+        <f t="shared" ref="R4:R21" si="7">M4^2</f>
         <v>1.7703002770083194</v>
       </c>
-    </row>
-    <row r="5" spans="2:18">
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T21" si="8">S4*C4</f>
+        <v>65.06</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ref="U4:U21" si="9">S4*C4*C4</f>
+        <v>2116.4018000000001</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V22" si="10">(C4-$C$33)/$I$32</f>
+        <v>-1.060102050191243</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W21" si="11">C4*C4*C4</f>
+        <v>34423.275277000001</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X22" si="12">C4</f>
+        <v>32.53</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y22" si="13">C4</f>
+        <v>32.53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25">
       <c r="B5" s="1">
         <v>41386</v>
       </c>
@@ -1273,15 +1379,15 @@
         <v>32.39</v>
       </c>
       <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-5.0931205874034466</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>8.7628480001167937</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="2"/>
-        <v>-5.0931205874034466</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>8.7628480001167937</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
         <v>-1.7205263157894777</v>
       </c>
       <c r="N5">
@@ -1304,8 +1410,35 @@
         <f t="shared" si="7"/>
         <v>2.9602108033241135</v>
       </c>
-    </row>
-    <row r="6" spans="2:18">
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="8"/>
+        <v>96.42</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="9"/>
+        <v>3098.9387999999999</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="10"/>
+        <v>-1.3708360767702426</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="11"/>
+        <v>33199.964344000007</v>
+      </c>
+      <c r="X5">
+        <f>C33</f>
+        <v>33.860526315789478</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="13"/>
+        <v>32.14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25">
       <c r="B6" s="1">
         <v>41383</v>
       </c>
@@ -1328,15 +1461,15 @@
         <v>32.1</v>
       </c>
       <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-3.5154572633036967</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>5.3453452808865203</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="2"/>
-        <v>-3.5154572633036967</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>5.3453452808865203</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
         <v>-1.5205263157894748</v>
       </c>
       <c r="N6">
@@ -1359,8 +1492,35 @@
         <f t="shared" si="7"/>
         <v>2.3120002770083139</v>
       </c>
-    </row>
-    <row r="7" spans="2:18">
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="8"/>
+        <v>129.36000000000001</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="9"/>
+        <v>4183.5024000000012</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="10"/>
+        <v>-1.2114852939092151</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="11"/>
+        <v>33823.616904000017</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="12"/>
+        <v>32.340000000000003</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="13"/>
+        <v>32.340000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25">
       <c r="B7" s="1">
         <v>41382</v>
       </c>
@@ -1383,15 +1543,15 @@
         <v>31.9</v>
       </c>
       <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-2.8063612771541142</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>3.9584464330384397</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="2"/>
-        <v>-2.8063612771541142</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>3.9584464330384397</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
         <v>-1.4105263157894754</v>
       </c>
       <c r="N7">
@@ -1414,8 +1574,35 @@
         <f t="shared" si="7"/>
         <v>1.9895844875346309</v>
       </c>
-    </row>
-    <row r="8" spans="2:18">
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="8"/>
+        <v>162.25</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="9"/>
+        <v>5265.0125000000007</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="10"/>
+        <v>-1.1238423633356518</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="11"/>
+        <v>34169.93112500001</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="12"/>
+        <v>32.450000000000003</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="13"/>
+        <v>32.450000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25">
       <c r="B8" s="1">
         <v>41381</v>
       </c>
@@ -1438,15 +1625,15 @@
         <v>32.46</v>
       </c>
       <c r="J8">
+        <f t="shared" si="0"/>
+        <v>-10.085064532001823</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>21.789047317825045</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="2"/>
-        <v>-10.085064532001823</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>21.789047317825045</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="1"/>
         <v>-2.160526315789479</v>
       </c>
       <c r="N8">
@@ -1469,8 +1656,35 @@
         <f t="shared" si="7"/>
         <v>4.6678739612188593</v>
       </c>
-    </row>
-    <row r="9" spans="2:18">
+      <c r="S8">
+        <v>6</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="8"/>
+        <v>190.2</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="9"/>
+        <v>6029.3399999999992</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="10"/>
+        <v>-1.7214077990644987</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="11"/>
+        <v>31855.012999999999</v>
+      </c>
+      <c r="X8">
+        <f>C33</f>
+        <v>33.860526315789478</v>
+      </c>
+      <c r="Y8">
+        <f>Y5</f>
+        <v>32.14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25">
       <c r="B9" s="1">
         <v>41380</v>
       </c>
@@ -1493,15 +1707,15 @@
         <v>32.33</v>
       </c>
       <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-0.53247762064442339</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.43158712410127342</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="2"/>
-        <v>-0.53247762064442339</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>0.43158712410127342</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
         <v>-0.81052631578948109</v>
       </c>
       <c r="N9">
@@ -1524,8 +1738,35 @@
         <f t="shared" si="7"/>
         <v>0.65695290858726962</v>
       </c>
-    </row>
-    <row r="10" spans="2:18">
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="8"/>
+        <v>231.34999999999997</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="9"/>
+        <v>7646.1174999999985</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="10"/>
+        <v>-0.64579001475258113</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="11"/>
+        <v>36100.597624999988</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="12"/>
+        <v>33.049999999999997</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="13"/>
+        <v>33.049999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25">
       <c r="B10" s="1">
         <v>41379</v>
       </c>
@@ -1548,15 +1789,15 @@
         <v>32.46</v>
       </c>
       <c r="J10">
+        <f t="shared" si="0"/>
+        <v>-2.9942994605629786E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>9.2980877985905236E-3</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="2"/>
-        <v>-2.9942994605629786E-2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>9.2980877985905236E-3</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="1"/>
         <v>-0.31052631578948109</v>
       </c>
       <c r="N10">
@@ -1579,8 +1820,35 @@
         <f t="shared" si="7"/>
         <v>9.6426592797788535E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:18">
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="8"/>
+        <v>268.39999999999998</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="9"/>
+        <v>9004.8199999999979</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="10"/>
+        <v>-0.2474130576000185</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="11"/>
+        <v>37763.963874999987</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="12"/>
+        <v>33.549999999999997</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="13"/>
+        <v>33.549999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25">
       <c r="B11" s="1">
         <v>41376</v>
       </c>
@@ -1603,15 +1871,15 @@
         <v>34.58</v>
       </c>
       <c r="J11">
+        <f t="shared" si="0"/>
+        <v>1.7469479078581446E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>4.5328700977581137E-3</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="2"/>
-        <v>1.7469479078581446E-2</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>4.5328700977581137E-3</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
         <v>0.2594736842105192</v>
       </c>
       <c r="N11">
@@ -1634,8 +1902,35 @@
         <f t="shared" si="7"/>
         <v>6.7326592797780235E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:18">
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="8"/>
+        <v>307.08</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="9"/>
+        <v>10477.569599999999</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="10"/>
+        <v>0.20673667355390316</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="11"/>
+        <v>39721.630527999994</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="12"/>
+        <v>34.119999999999997</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="13"/>
+        <v>34.119999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25">
       <c r="B12" s="1">
         <v>41375</v>
       </c>
@@ -1658,15 +1953,15 @@
         <v>34.14</v>
       </c>
       <c r="J12">
+        <f t="shared" si="0"/>
+        <v>2.1440625455605473</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>2.7647122298017455</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="2"/>
-        <v>2.1440625455605473</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>2.7647122298017455</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
         <v>1.2894736842105203</v>
       </c>
       <c r="N12">
@@ -1689,8 +1984,35 @@
         <f t="shared" si="7"/>
         <v>1.6627423822714527</v>
       </c>
-    </row>
-    <row r="13" spans="2:18">
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="8"/>
+        <v>351.5</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="9"/>
+        <v>12355.225</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="10"/>
+        <v>1.0273932052881831</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="11"/>
+        <v>43428.615874999989</v>
+      </c>
+      <c r="X12">
+        <f>C33</f>
+        <v>33.860526315789478</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="13"/>
+        <v>35.15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25">
       <c r="B13" s="1">
         <v>41374</v>
       </c>
@@ -1713,15 +2035,15 @@
         <v>35</v>
       </c>
       <c r="J13">
+        <f t="shared" si="0"/>
+        <v>16.964166346114496</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>43.588979000910953</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="2"/>
-        <v>16.964166346114496</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>43.588979000910953</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
         <v>2.5694736842105215</v>
       </c>
       <c r="N13">
@@ -1744,8 +2066,35 @@
         <f t="shared" si="7"/>
         <v>6.6021950138503902</v>
       </c>
-    </row>
-    <row r="14" spans="2:18">
+      <c r="S13">
+        <v>11</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="8"/>
+        <v>400.73</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="9"/>
+        <v>14598.5939</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="10"/>
+        <v>2.0472382155987443</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="11"/>
+        <v>48347.888706999998</v>
+      </c>
+      <c r="X13">
+        <f>C33</f>
+        <v>33.860526315789478</v>
+      </c>
+      <c r="Y13">
+        <f>Y12</f>
+        <v>35.15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25">
       <c r="B14" s="1">
         <v>41373</v>
       </c>
@@ -1768,15 +2117,15 @@
         <v>36.19</v>
       </c>
       <c r="J14">
+        <f t="shared" si="0"/>
+        <v>1.4794929472226095</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>1.6858432793352298</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="2"/>
-        <v>1.4794929472226095</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>1.6858432793352298</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
         <v>1.1394736842105218</v>
       </c>
       <c r="N14">
@@ -1799,8 +2148,35 @@
         <f t="shared" si="7"/>
         <v>1.2984002770082999</v>
       </c>
-    </row>
-    <row r="15" spans="2:18">
+      <c r="S14">
+        <v>12</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="8"/>
+        <v>420</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="9"/>
+        <v>14700</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="10"/>
+        <v>0.90788011814241543</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="11"/>
+        <v>42875</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="12"/>
+        <v>35</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="13"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25">
       <c r="B15" s="1">
         <v>41372</v>
       </c>
@@ -1823,15 +2199,15 @@
         <v>34.700000000000003</v>
       </c>
       <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.57069995276277929</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0.47338059239691194</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="2"/>
-        <v>0.57069995276277929</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>0.47338059239691194</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
         <v>0.82947368421051948</v>
       </c>
       <c r="N15">
@@ -1854,8 +2230,35 @@
         <f t="shared" si="7"/>
         <v>0.68802659279777256</v>
       </c>
-    </row>
-    <row r="16" spans="2:18">
+      <c r="S15">
+        <v>13</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="8"/>
+        <v>450.96999999999997</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="9"/>
+        <v>15644.149299999997</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="10"/>
+        <v>0.66088640470782478</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="11"/>
+        <v>41745.810708999998</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="12"/>
+        <v>34.69</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="13"/>
+        <v>34.69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25">
       <c r="B16" s="1">
         <v>41369</v>
       </c>
@@ -1878,15 +2281,15 @@
         <v>34.56</v>
       </c>
       <c r="J16">
+        <f t="shared" si="0"/>
+        <v>-1.7508367108909125E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>2.1102189831264607E-4</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="2"/>
-        <v>-1.7508367108909125E-3</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>2.1102189831264607E-4</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="1"/>
         <v>-0.12052631578947626</v>
       </c>
       <c r="N16">
@@ -1909,8 +2312,35 @@
         <f t="shared" si="7"/>
         <v>1.4526592797784553E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16">
+        <v>14</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="8"/>
+        <v>472.36</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="9"/>
+        <v>15937.426400000002</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="10"/>
+        <v>-9.6029813882040835E-2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="11"/>
+        <v>38409.197624000008</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="12"/>
+        <v>33.74</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="13"/>
+        <v>33.74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="B17" s="1">
         <v>41368</v>
       </c>
@@ -1933,15 +2363,15 @@
         <v>34.19</v>
       </c>
       <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1.2931539583029534</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>1.408857207203742</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="2"/>
-        <v>1.2931539583029534</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>1.408857207203742</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="1"/>
         <v>1.0894736842105246</v>
       </c>
       <c r="N17">
@@ -1964,8 +2394,35 @@
         <f t="shared" si="7"/>
         <v>1.1869529085872539</v>
       </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17">
+        <v>15</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="8"/>
+        <v>524.25</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="9"/>
+        <v>18322.537500000002</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="10"/>
+        <v>0.86804242242716145</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="11"/>
+        <v>42691.512375000013</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="12"/>
+        <v>34.950000000000003</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="13"/>
+        <v>34.950000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="B18" s="1">
         <v>41367</v>
       </c>
@@ -1988,15 +2445,15 @@
         <v>35.159999999999997</v>
       </c>
       <c r="J18">
+        <f t="shared" si="0"/>
+        <v>-0.3151626705059114</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>0.21447649103376121</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="2"/>
-        <v>-0.3151626705059114</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>0.21447649103376121</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="1"/>
         <v>-0.68052631578947853</v>
       </c>
       <c r="N18">
@@ -2019,8 +2476,35 @@
         <f t="shared" si="7"/>
         <v>0.46311606648200104</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18">
+        <v>16</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="8"/>
+        <v>530.88</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="9"/>
+        <v>17614.598399999999</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="10"/>
+        <v>-0.54221200589291285</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="11"/>
+        <v>36528.273431999995</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="12"/>
+        <v>33.18</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="13"/>
+        <v>33.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="B19" s="1">
         <v>41366</v>
       </c>
@@ -2043,15 +2527,15 @@
         <v>33.25</v>
       </c>
       <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0.85595078932788415</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>0.81270274944605236</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="2"/>
-        <v>0.85595078932788415</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>0.81270274944605236</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="1"/>
         <v>0.94947368421052403</v>
       </c>
       <c r="N19">
@@ -2074,8 +2558,35 @@
         <f t="shared" si="7"/>
         <v>0.90150027700830593</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19">
+        <v>17</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="8"/>
+        <v>591.77</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="9"/>
+        <v>20599.5137</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="10"/>
+        <v>0.75649687442444347</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="11"/>
+        <v>42180.533641000009</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="12"/>
+        <v>34.81</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="13"/>
+        <v>34.81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="B20" s="1">
         <v>41365</v>
       </c>
@@ -2098,15 +2609,15 @@
         <v>34</v>
       </c>
       <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0.85595078932788415</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>0.81270274944605236</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="2"/>
-        <v>0.85595078932788415</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>0.81270274944605236</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="1"/>
         <v>0.94947368421052403</v>
       </c>
       <c r="N20">
@@ -2129,8 +2640,35 @@
         <f t="shared" si="7"/>
         <v>0.90150027700830593</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20">
+        <v>18</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="8"/>
+        <v>626.58000000000004</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="9"/>
+        <v>21811.249800000001</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="10"/>
+        <v>0.75649687442444347</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="11"/>
+        <v>42180.533641000009</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="12"/>
+        <v>34.81</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="13"/>
+        <v>34.81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="B21" s="1">
         <v>41362</v>
       </c>
@@ -2153,15 +2691,15 @@
         <v>35.130000000000003</v>
       </c>
       <c r="J21">
+        <f t="shared" si="0"/>
+        <v>2.0458373710453324</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>2.5971367047164917</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="2"/>
-        <v>2.0458373710453324</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>2.5971367047164917</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="1"/>
         <v>1.2694736842105243</v>
       </c>
       <c r="N21">
@@ -2184,8 +2722,35 @@
         <f t="shared" si="7"/>
         <v>1.6115634349030421</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21">
+        <v>19</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="8"/>
+        <v>667.47</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="9"/>
+        <v>23448.221100000002</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="10"/>
+        <v>1.0114581270020837</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="11"/>
+        <v>43354.526697000008</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="12"/>
+        <v>35.130000000000003</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="13"/>
+        <v>35.130000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="J22">
         <f>SUM(J3:J21)/19</f>
         <v>7.7365224668300134E-2</v>
@@ -2195,47 +2760,75 @@
         <v>5.1473822692649636</v>
       </c>
       <c r="P22">
-        <f>SUM(P3:P21)</f>
+        <f t="shared" ref="P22:U22" si="14">SUM(P3:P21)</f>
         <v>0.56189736435595405</v>
       </c>
       <c r="Q22">
-        <f>SUM(Q3:Q21)</f>
+        <f t="shared" si="14"/>
         <v>66.90969033519778</v>
       </c>
       <c r="R22">
-        <f>SUM(R3:R21)</f>
+        <f t="shared" si="14"/>
         <v>29.929894736842112</v>
       </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22">
+        <f t="shared" si="14"/>
+        <v>190</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="14"/>
+        <v>6520.21</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="14"/>
+        <v>223980.83409999998</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="10"/>
+        <v>-26.978506882536969</v>
+      </c>
+      <c r="W22">
+        <f>SUM(W3:W21)</f>
+        <v>740665.24409100006</v>
+      </c>
+      <c r="X22">
+        <f>AVERAGE(X3:X21)</f>
+        <v>33.861689750692513</v>
+      </c>
+      <c r="Y22">
+        <f>AVERAGE(Y3:Y21)</f>
+        <v>33.816315789473677</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="O23">
         <f>SUM(O3:O22)</f>
         <v>27.299131578947375</v>
       </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="T23">
+        <f>T22/S22</f>
+        <v>34.316894736842109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="e">
-        <f>CORREL(C3:C21,C13:C21)</f>
-        <v>#N/A</v>
+        <v>47</v>
       </c>
       <c r="G24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I24">
         <f>O24</f>
         <v>1.5166184210526319</v>
       </c>
       <c r="M24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N24" s="2">
         <f>(1/18)</f>
@@ -2246,459 +2839,523 @@
         <v>1.5166184210526319</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <f>CORREL(C3:C21,D3:D21)</f>
         <v>0.88543622453699311</v>
       </c>
       <c r="G25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I25">
         <f>SQRT((24*19*18*18/(16*17*22*24)))</f>
         <v>1.0142698435367294</v>
       </c>
-      <c r="J25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="J25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <f>COVAR(C3:C21,D3:D21)</f>
         <v>1.436796398891967</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I26">
         <f>SKEW(C3:C21)</f>
         <v>4.2567930807993273E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
+      <c r="C27">
+        <f>SUMXMY2(C4:C21,C3:C20)/SUMSQ(C3:C21)</f>
+        <v>7.9607686762407995E-4</v>
+      </c>
       <c r="G27" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I27">
         <f>SQRT(6*19*18/(17*20*22))</f>
         <v>0.52376669501042072</v>
       </c>
-      <c r="J27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="J27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
+      <c r="C28">
+        <f>GEOMEAN(C3:C21)</f>
+        <v>33.837262944797303</v>
+      </c>
       <c r="G28" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J28">
         <f>STDEV(C3:C21)</f>
         <v>1.2894851413741388</v>
       </c>
       <c r="K28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="C29">
-        <f>GEOMEAN(C3:C21)</f>
-        <v>33.837262944797303</v>
+        <f>HARMEAN(C3:C21)</f>
+        <v>33.814004487772912</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I29">
         <f>VARA(C3:C21)</f>
         <v>1.6627719298246828</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30">
-        <f>HARMEAN(C3:C21)</f>
-        <v>33.814004487772912</v>
+        <f>L2</f>
+        <v>-0.92564422252414147</v>
+      </c>
+      <c r="G30" t="s">
+        <v>48</v>
       </c>
       <c r="H30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
+        <v>45</v>
+      </c>
+      <c r="I30">
+        <f>(I46-I45*I45/S22)/(S22-1)</f>
+        <v>1.2035654385963137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="C31">
-        <f>L2</f>
-        <v>-0.92564422252414147</v>
-      </c>
       <c r="G31" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I31">
-        <f>C39/(I33*I33*I33)</f>
+        <f>C38/(I32*I32*I32)</f>
         <v>3.9130771304849168E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
+      <c r="C32">
+        <f>MAX(C3:C21)</f>
+        <v>36.43</v>
+      </c>
+      <c r="G32" t="s">
+        <v>48</v>
+      </c>
       <c r="H32" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="I32">
+        <f>STDEVPA(C3:C21)</f>
+        <v>1.2550926729643144</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
       </c>
       <c r="C33">
-        <f>MAX(C3:C21)</f>
-        <v>36.43</v>
+        <f>AVERAGE(C3:C21)</f>
+        <v>33.860526315789478</v>
       </c>
       <c r="G33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I33">
-        <f>STDEVPA(C3:C21)</f>
-        <v>1.2550926729643144</v>
+        <f>SQRT(I42/19)</f>
+        <v>0.28793800664367314</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
       </c>
       <c r="C34">
-        <f>AVERAGE(C3:C21)</f>
-        <v>33.860526315789478</v>
-      </c>
-      <c r="D34">
+        <f>AVEDEV(C3:C21)</f>
+        <v>1.0889750692520779</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34">
+        <f>SUM(C3:C21)</f>
+        <v>643.35</v>
+      </c>
+      <c r="J34">
+        <f>STDEVPA(D3:D21)</f>
+        <v>1.2928917104959985</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <f>MEDIAN(C3:C21)</f>
+        <v>33.74</v>
+      </c>
+      <c r="D35">
         <f>AVERAGE(D3:D21)</f>
         <v>34.486842105263158</v>
       </c>
-      <c r="G34" t="s">
-        <v>53</v>
-      </c>
-      <c r="H34" t="s">
-        <v>43</v>
-      </c>
-      <c r="I34">
-        <f>SQRT(I44/19)</f>
-        <v>0.28793800664367314</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35">
-        <f>AVEDEV(C3:C21)</f>
-        <v>1.0889750692520779</v>
+      <c r="G35" t="s">
+        <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>44</v>
-      </c>
-      <c r="J35">
-        <f>STDEVPA(D3:D21)</f>
-        <v>1.2928917104959985</v>
+        <v>42</v>
+      </c>
+      <c r="I35">
+        <f>P22</f>
+        <v>0.56189736435595405</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
       </c>
       <c r="C36">
-        <f>MEDIAN(C3:C21)</f>
-        <v>33.74</v>
+        <f>MIN(C3:C21)</f>
+        <v>31.7</v>
       </c>
       <c r="G36" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I36">
-        <f>SUM(C3:C21)</f>
-        <v>643.35</v>
+        <f>Q22</f>
+        <v>66.90969033519778</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" t="s">
-        <v>53</v>
-      </c>
       <c r="B37" t="s">
         <v>17</v>
       </c>
-      <c r="C37">
-        <f>MIN(C3:C21)</f>
-        <v>31.7</v>
-      </c>
       <c r="G37" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H37" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="I37">
-        <f>P22</f>
-        <v>0.56189736435595405</v>
+        <f>R22</f>
+        <v>29.929894736842112</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
+      <c r="C38">
+        <f>J22</f>
+        <v>7.7365224668300134E-2</v>
+      </c>
       <c r="G38" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="I38">
-        <f>Q22</f>
-        <v>66.90969033519778</v>
+        <f>W22</f>
+        <v>740665.24409100006</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39">
-        <f>J22</f>
-        <v>7.7365224668300134E-2</v>
+        <f>K22</f>
+        <v>5.1473822692649636</v>
+      </c>
+      <c r="G39" t="s">
+        <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="I39">
-        <f>R22</f>
-        <v>29.929894736842112</v>
+        <f>SUMSQ(C3:C21)</f>
+        <v>21814.099500000004</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
       </c>
       <c r="C40">
-        <f>K22</f>
-        <v>5.1473822692649636</v>
+        <f>(19*C33+19*D35)/(19+19)</f>
+        <v>34.173684210526318</v>
+      </c>
+      <c r="G40" t="s">
+        <v>48</v>
       </c>
       <c r="H40" t="s">
-        <v>71</v>
+        <v>33</v>
+      </c>
+      <c r="I40">
+        <f>I42*18</f>
+        <v>28.354637119116731</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>21</v>
       </c>
       <c r="C41">
-        <f>(19*C34+19*D34)/(19+19)</f>
-        <v>34.173684210526318</v>
+        <f>(19*I42+19*J45)/(19+19)</f>
+        <v>1.623413296398988</v>
       </c>
       <c r="G41" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H41" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="I41">
-        <f>SUMSQ(C3:C21)</f>
-        <v>21814.099500000004</v>
+        <f>X22</f>
+        <v>33.861689750692513</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
         <v>22</v>
       </c>
       <c r="C42">
-        <f>(19*I44+19*J46)/(19+19)</f>
-        <v>1.623413296398988</v>
+        <f>PRODUCT(C3:C21)</f>
+        <v>1.144219377783957E+29</v>
+      </c>
+      <c r="G42" t="s">
+        <v>48</v>
       </c>
       <c r="H42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I42">
-        <f>DEVSQ(C3:C21)</f>
-        <v>29.929894736842112</v>
+        <f>VARP(C3:C21)</f>
+        <v>1.5752576177287072</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
       </c>
       <c r="C43">
-        <f>PRODUCT(C3:C21)</f>
-        <v>1.144219377783957E+29</v>
+        <f>PERCENTILE(C3:C21,20%)</f>
+        <v>32.498000000000005</v>
+      </c>
+      <c r="G43" t="s">
+        <v>48</v>
       </c>
       <c r="H43" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="I43">
+        <f>T23</f>
+        <v>34.316894736842109</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C44">
-        <f>PERCENTILE(C3:C21,20%)</f>
-        <v>32.498000000000005</v>
-      </c>
-      <c r="G44" t="s">
-        <v>53</v>
+        <f>16/19</f>
+        <v>0.84210526315789469</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="I44">
-        <f>VARP(C3:C21)</f>
-        <v>1.5752576177287072</v>
+        <f>I45/I46</f>
+        <v>2.9110571117388302E-2</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45">
-        <f>16/19</f>
-        <v>0.84210526315789469</v>
+        <v>24</v>
+      </c>
+      <c r="G45" t="s">
+        <v>48</v>
       </c>
       <c r="H45" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="I45">
+        <f>T22</f>
+        <v>6520.21</v>
+      </c>
+      <c r="J45">
+        <f>VARP(D3:D21)</f>
+        <v>1.6715689750692686</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
       </c>
+      <c r="C46">
+        <f>SQRT(I39/19)</f>
+        <v>33.883779305148359</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
+      </c>
       <c r="H46" t="s">
-        <v>50</v>
-      </c>
-      <c r="J46">
-        <f>VARP(D3:D21)</f>
-        <v>1.6715689750692686</v>
+        <v>67</v>
+      </c>
+      <c r="I46">
+        <f>U22</f>
+        <v>223980.83409999998</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
         <v>26</v>
       </c>
       <c r="C47">
-        <f>SQRT(I41/19)</f>
-        <v>33.883779305148359</v>
-      </c>
-      <c r="H47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48">
         <f>KURT(C3:C21)</f>
         <v>-0.8280585298107539</v>
+      </c>
+      <c r="G47" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" t="s">
+        <v>36</v>
+      </c>
+      <c r="I47">
+        <f>Y22</f>
+        <v>33.816315789473677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>